<commit_message>
worked on some bug fix with cleaning up strings before we search through things. Also added a command list
</commit_message>
<xml_diff>
--- a/NSguildresponses.xlsx
+++ b/NSguildresponses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
   <si>
     <t>0</t>
   </si>
@@ -52,7 +52,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>2026-01-01 12:13:01</t>
+    <t>2026-01-07 17:27:34</t>
   </si>
   <si>
     <t>2025-12-25 02:45:26</t>
@@ -121,7 +121,7 @@
     <t>2025-12-25 13:18:12</t>
   </si>
   <si>
-    <t>2026-01-01 15:19:02</t>
+    <t>2026-01-07 22:29:11</t>
   </si>
   <si>
     <t>2025-12-29 18:10:26</t>
@@ -130,9 +130,6 @@
     <t>2026-01-04 20:17:17</t>
   </si>
   <si>
-    <t>2026-01-03 14:45:48</t>
-  </si>
-  <si>
     <t>2026-01-03 17:08:10</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>flyingbeast223</t>
   </si>
   <si>
-    <t>partykat</t>
-  </si>
-  <si>
     <t>Ryuden</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>Ooflegend</t>
   </si>
   <si>
-    <t>PartyKat</t>
-  </si>
-  <si>
     <t>Segwarides</t>
   </si>
   <si>
@@ -547,7 +538,7 @@
     <t>Offense, Scout</t>
   </si>
   <si>
-    <t>Defense, Flex, Cannoneer, Scout, Shotcaller</t>
+    <t>Offense, Defense, Flex, Scout, Shotcaller</t>
   </si>
   <si>
     <t>Offense, Flex, Cannoneer</t>
@@ -944,7 +935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -993,13 +984,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2">
         <v>392</v>
@@ -1008,22 +999,22 @@
         <v>388</v>
       </c>
       <c r="G2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L2">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1031,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E3">
         <v>322</v>
@@ -1049,16 +1040,16 @@
         <v>424</v>
       </c>
       <c r="H3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L3">
         <v>751</v>
@@ -1069,13 +1060,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>351</v>
@@ -1087,16 +1078,16 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L4">
         <v>780</v>
@@ -1107,13 +1098,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E5">
         <v>347</v>
@@ -1125,16 +1116,16 @@
         <v>426</v>
       </c>
       <c r="H5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L5">
         <v>773</v>
@@ -1145,13 +1136,13 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E6">
         <v>355</v>
@@ -1163,16 +1154,16 @@
         <v>425</v>
       </c>
       <c r="H6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L6">
         <v>780</v>
@@ -1183,13 +1174,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7">
         <v>372</v>
@@ -1201,16 +1192,16 @@
         <v>442</v>
       </c>
       <c r="H7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L7">
         <v>814</v>
@@ -1221,13 +1212,13 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E8">
         <v>358</v>
@@ -1239,16 +1230,16 @@
         <v>428</v>
       </c>
       <c r="H8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L8">
         <v>794</v>
@@ -1259,13 +1250,13 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E9">
         <v>332</v>
@@ -1277,16 +1268,16 @@
         <v>427</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L9">
         <v>761</v>
@@ -1297,13 +1288,13 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E10">
         <v>355</v>
@@ -1315,16 +1306,16 @@
         <v>416</v>
       </c>
       <c r="H10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L10">
         <v>771</v>
@@ -1335,13 +1326,13 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E11">
         <v>381</v>
@@ -1353,16 +1344,16 @@
         <v>454</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L11">
         <v>841</v>
@@ -1373,13 +1364,13 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E12">
         <v>354</v>
@@ -1391,16 +1382,16 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L12">
         <v>781</v>
@@ -1411,13 +1402,13 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E13">
         <v>285</v>
@@ -1429,16 +1420,16 @@
         <v>379</v>
       </c>
       <c r="H13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L13">
         <v>666</v>
@@ -1449,13 +1440,13 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E14">
         <v>364</v>
@@ -1467,16 +1458,16 @@
         <v>434</v>
       </c>
       <c r="H14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L14">
         <v>798</v>
@@ -1487,13 +1478,13 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E15">
         <v>389</v>
@@ -1505,16 +1496,16 @@
         <v>460</v>
       </c>
       <c r="H15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L15">
         <v>849</v>
@@ -1525,13 +1516,13 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E16">
         <v>393</v>
@@ -1543,16 +1534,16 @@
         <v>463</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L16">
         <v>858</v>
@@ -1563,13 +1554,13 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E17">
         <v>389</v>
@@ -1581,16 +1572,16 @@
         <v>459</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L17">
         <v>852</v>
@@ -1601,13 +1592,13 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E18">
         <v>282</v>
@@ -1619,16 +1610,16 @@
         <v>369</v>
       </c>
       <c r="H18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L18">
         <v>651</v>
@@ -1639,13 +1630,13 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E19">
         <v>256</v>
@@ -1657,16 +1648,16 @@
         <v>317</v>
       </c>
       <c r="H19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L19">
         <v>583</v>
@@ -1677,13 +1668,13 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E20">
         <v>390</v>
@@ -1695,16 +1686,16 @@
         <v>459</v>
       </c>
       <c r="H20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L20">
         <v>849</v>
@@ -1715,13 +1706,13 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E21">
         <v>374</v>
@@ -1733,16 +1724,16 @@
         <v>447</v>
       </c>
       <c r="H21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L21">
         <v>821</v>
@@ -1753,13 +1744,13 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E22">
         <v>365</v>
@@ -1771,16 +1762,16 @@
         <v>432</v>
       </c>
       <c r="H22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L22">
         <v>803</v>
@@ -1791,13 +1782,13 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E23">
         <v>365</v>
@@ -1809,16 +1800,16 @@
         <v>413</v>
       </c>
       <c r="H23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L23">
         <v>778</v>
@@ -1829,13 +1820,13 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E24">
         <v>386</v>
@@ -1847,16 +1838,16 @@
         <v>462</v>
       </c>
       <c r="H24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L24">
         <v>856</v>
@@ -1867,13 +1858,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="E25">
         <v>363</v>
@@ -1882,22 +1873,22 @@
         <v>363</v>
       </c>
       <c r="G25">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L25">
-        <v>797</v>
+        <v>804</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1905,13 +1896,13 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E26">
         <v>369</v>
@@ -1923,16 +1914,16 @@
         <v>446</v>
       </c>
       <c r="H26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I26" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L26">
         <v>821</v>
@@ -1943,13 +1934,13 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E27">
         <v>367</v>
@@ -1961,16 +1952,16 @@
         <v>437</v>
       </c>
       <c r="H27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I27" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J27" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L27">
         <v>804</v>
@@ -1981,37 +1972,37 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="E28">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="F28">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="G28">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="H28" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I28" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K28" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L28">
-        <v>789</v>
+        <v>838</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2019,37 +2010,37 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E29">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="F29">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G29">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="H29" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="I29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J29" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L29">
-        <v>838</v>
+        <v>815</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2057,37 +2048,37 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E30">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="F30">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="G30">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I30" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J30" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K30" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L30">
-        <v>815</v>
+        <v>798</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2095,37 +2086,37 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E31">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="F31">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="G31">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="I31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L31">
-        <v>798</v>
+        <v>823</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2133,37 +2124,37 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E32">
-        <v>369</v>
+        <v>279</v>
       </c>
       <c r="F32">
-        <v>373</v>
+        <v>291</v>
       </c>
       <c r="G32">
-        <v>450</v>
+        <v>360</v>
       </c>
       <c r="H32" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="I32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L32">
-        <v>823</v>
+        <v>651</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2171,37 +2162,37 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E33">
-        <v>279</v>
+        <v>373</v>
       </c>
       <c r="F33">
-        <v>291</v>
+        <v>375</v>
       </c>
       <c r="G33">
-        <v>360</v>
+        <v>451</v>
       </c>
       <c r="H33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I33" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J33" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K33" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L33">
-        <v>651</v>
+        <v>826</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2209,37 +2200,37 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E34">
+        <v>379</v>
+      </c>
+      <c r="F34">
         <v>373</v>
       </c>
-      <c r="F34">
-        <v>375</v>
-      </c>
       <c r="G34">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="H34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I34" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J34" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L34">
-        <v>826</v>
+        <v>819</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2247,37 +2238,37 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E35">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F35">
-        <v>373</v>
+        <v>389</v>
       </c>
       <c r="G35">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="H35" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L35">
-        <v>819</v>
+        <v>840</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2285,37 +2276,37 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E36">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="F36">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G36">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="H36" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L36">
-        <v>840</v>
+        <v>850</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2323,37 +2314,37 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E37">
-        <v>390</v>
+        <v>358</v>
       </c>
       <c r="F37">
-        <v>390</v>
+        <v>358</v>
       </c>
       <c r="G37">
-        <v>460</v>
+        <v>428</v>
       </c>
       <c r="H37" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="I37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K37" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L37">
-        <v>850</v>
+        <v>786</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2361,37 +2352,37 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="E38">
-        <v>358</v>
+        <v>305</v>
       </c>
       <c r="F38">
-        <v>358</v>
+        <v>307</v>
       </c>
       <c r="G38">
-        <v>428</v>
+        <v>375</v>
       </c>
       <c r="H38" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="I38" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J38" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K38" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L38">
-        <v>786</v>
+        <v>682</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2399,37 +2390,37 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="E39">
-        <v>305</v>
+        <v>367</v>
       </c>
       <c r="F39">
-        <v>307</v>
+        <v>371</v>
       </c>
       <c r="G39">
-        <v>375</v>
+        <v>438</v>
       </c>
       <c r="H39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I39" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J39" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K39" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L39">
-        <v>682</v>
+        <v>809</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2437,37 +2428,37 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="E40">
-        <v>367</v>
+        <v>332</v>
       </c>
       <c r="F40">
-        <v>371</v>
+        <v>316</v>
       </c>
       <c r="G40">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="H40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I40" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J40" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L40">
-        <v>809</v>
+        <v>759</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2475,37 +2466,37 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="E41">
-        <v>332</v>
+        <v>374</v>
       </c>
       <c r="F41">
-        <v>316</v>
+        <v>380</v>
       </c>
       <c r="G41">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="H41" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="I41" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J41" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L41">
-        <v>759</v>
+        <v>823</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2513,37 +2504,37 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="E42">
         <v>374</v>
       </c>
       <c r="F42">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="G42">
         <v>443</v>
       </c>
       <c r="H42" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I42" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J42" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K42" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L42">
-        <v>823</v>
+        <v>817</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2551,37 +2542,37 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E43">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F43">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="G43">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="H43" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="I43" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K43" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L43">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2589,37 +2580,37 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E44">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="F44">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="G44">
-        <v>438</v>
+        <v>416</v>
       </c>
       <c r="H44" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="I44" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J44" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K44" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L44">
-        <v>818</v>
+        <v>758</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2627,37 +2618,37 @@
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="E45">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="F45">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="G45">
-        <v>416</v>
+        <v>314</v>
       </c>
       <c r="H45" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L45">
-        <v>758</v>
+        <v>636</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2665,37 +2656,37 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E46">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="F46">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="G46">
-        <v>314</v>
+        <v>411</v>
       </c>
       <c r="H46" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="I46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K46" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L46">
-        <v>636</v>
+        <v>749</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2703,74 +2694,36 @@
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E47">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="F47">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="G47">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="H47" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="I47" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J47" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K47" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L47">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E48">
-        <v>358</v>
-      </c>
-      <c r="F48">
-        <v>358</v>
-      </c>
-      <c r="G48">
-        <v>434</v>
-      </c>
-      <c r="H48" t="s">
-        <v>188</v>
-      </c>
-      <c r="I48" t="s">
-        <v>189</v>
-      </c>
-      <c r="J48" t="s">
-        <v>189</v>
-      </c>
-      <c r="K48" t="s">
-        <v>190</v>
-      </c>
-      <c r="L48">
         <v>792</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new features such as rmplayer and noobslum
</commit_message>
<xml_diff>
--- a/NSguildresponses.xlsx
+++ b/NSguildresponses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="228">
   <si>
     <t>0</t>
   </si>
@@ -52,7 +52,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>2026-01-07 17:27:34</t>
+    <t>2026-01-21 17:20:55</t>
   </si>
   <si>
     <t>2025-12-25 02:45:26</t>
@@ -61,31 +61,37 @@
     <t>2026-01-01 17:20:47</t>
   </si>
   <si>
+    <t>2026-01-10 10:53:18</t>
+  </si>
+  <si>
     <t>2026-01-03 17:36:51</t>
   </si>
   <si>
-    <t>2026-01-01 11:34:46</t>
-  </si>
-  <si>
-    <t>2026-01-01 21:25:11</t>
-  </si>
-  <si>
-    <t>2026-01-01 22:01:52</t>
-  </si>
-  <si>
-    <t>2026-01-05 22:33:02</t>
-  </si>
-  <si>
-    <t>2026-01-06 17:31:44</t>
-  </si>
-  <si>
-    <t>2026-01-01 16:41:46</t>
-  </si>
-  <si>
-    <t>2026-01-03 22:09:38</t>
-  </si>
-  <si>
-    <t>2026-01-03 18:09:58</t>
+    <t>2026-01-17 09:32:37</t>
+  </si>
+  <si>
+    <t>2026-01-24 18:03:44</t>
+  </si>
+  <si>
+    <t>2026-01-23 20:26:16</t>
+  </si>
+  <si>
+    <t>2026-01-23 10:09:18</t>
+  </si>
+  <si>
+    <t>2026-01-15 20:59:10</t>
+  </si>
+  <si>
+    <t>2026-01-25 00:51:12</t>
+  </si>
+  <si>
+    <t>2026-01-23 00:05:33</t>
+  </si>
+  <si>
+    <t>2026-01-18 15:23:45</t>
+  </si>
+  <si>
+    <t>2026-01-11 21:18:53</t>
   </si>
   <si>
     <t>2026-01-03 06:43:45</t>
@@ -100,34 +106,52 @@
     <t>2026-01-06 16:38:25</t>
   </si>
   <si>
+    <t>2026-01-16 21:26:49</t>
+  </si>
+  <si>
     <t>2026-01-03 16:35:58</t>
   </si>
   <si>
+    <t>2026-01-10 00:59:56</t>
+  </si>
+  <si>
     <t>2026-01-03 15:13:48</t>
   </si>
   <si>
-    <t>2026-01-03 17:14:56</t>
-  </si>
-  <si>
-    <t>2025-12-25 02:49:59</t>
-  </si>
-  <si>
-    <t>2026-01-03 19:08:56</t>
-  </si>
-  <si>
-    <t>2026-01-04 00:02:20</t>
+    <t>2026-01-13 19:56:37</t>
+  </si>
+  <si>
+    <t>2026-01-24 17:55:28</t>
+  </si>
+  <si>
+    <t>2026-01-11 12:34:01</t>
+  </si>
+  <si>
+    <t>2026-01-25 13:35:17</t>
+  </si>
+  <si>
+    <t>2026-01-22 23:53:09</t>
+  </si>
+  <si>
+    <t>2026-01-23 00:12:53</t>
   </si>
   <si>
     <t>2025-12-25 13:18:12</t>
   </si>
   <si>
-    <t>2026-01-07 22:29:11</t>
+    <t>2026-01-21 16:47:55</t>
+  </si>
+  <si>
+    <t>2026-01-18 01:37:22</t>
   </si>
   <si>
     <t>2025-12-29 18:10:26</t>
   </si>
   <si>
-    <t>2026-01-04 20:17:17</t>
+    <t>2026-01-18 05:43:13</t>
+  </si>
+  <si>
+    <t>2026-01-10 10:43:03</t>
   </si>
   <si>
     <t>2026-01-03 17:08:10</t>
@@ -142,52 +166,67 @@
     <t>2026-01-01 18:14:04</t>
   </si>
   <si>
-    <t>2026-01-02 20:14:30</t>
-  </si>
-  <si>
     <t>2026-01-04 08:33:50</t>
   </si>
   <si>
     <t>2026-01-01 12:39:24</t>
   </si>
   <si>
-    <t>2026-01-01 17:12:31</t>
+    <t>2026-01-23 00:37:06</t>
+  </si>
+  <si>
+    <t>2026-01-18 15:22:06</t>
   </si>
   <si>
     <t>2026-01-01 10:34:09</t>
   </si>
   <si>
+    <t>2026-01-24 16:39:43</t>
+  </si>
+  <si>
+    <t>2026-01-16 22:27:31</t>
+  </si>
+  <si>
     <t>2026-01-01 10:30:44</t>
   </si>
   <si>
     <t>2026-01-06 05:11:07</t>
   </si>
   <si>
-    <t>2026-01-03 17:24:35</t>
+    <t>2026-01-09 16:50:26</t>
   </si>
   <si>
     <t>2026-01-01 16:13:47</t>
   </si>
   <si>
-    <t>2026-01-01 11:05:53</t>
-  </si>
-  <si>
-    <t>2025-12-25 02:47:39</t>
-  </si>
-  <si>
-    <t>2026-01-07 02:12:02</t>
-  </si>
-  <si>
-    <t>2026-01-01 17:46:11</t>
+    <t>2026-01-22 23:52:07</t>
+  </si>
+  <si>
+    <t>2026-01-25 01:54:10</t>
+  </si>
+  <si>
+    <t>2026-01-15 20:57:58</t>
+  </si>
+  <si>
+    <t>2026-01-25 07:55:59</t>
+  </si>
+  <si>
+    <t>2026-01-10 11:07:06</t>
   </si>
   <si>
     <t>2026-01-01 09:55:59</t>
   </si>
   <si>
+    <t>2026-01-08 12:53:53</t>
+  </si>
+  <si>
     <t>2026-01-06 00:00:55</t>
   </si>
   <si>
-    <t>2026-01-01 23:53:08</t>
+    <t>2026-01-10 11:21:25</t>
+  </si>
+  <si>
+    <t>2026-01-10 20:47:43</t>
   </si>
   <si>
     <t>acidfs</t>
@@ -199,19 +238,25 @@
     <t>banes</t>
   </si>
   <si>
+    <t>billberry</t>
+  </si>
+  <si>
     <t>biven</t>
   </si>
   <si>
-    <t>marwolaeth66</t>
-  </si>
-  <si>
-    <t>cairis</t>
+    <t>numer</t>
+  </si>
+  <si>
+    <t>Cairis</t>
   </si>
   <si>
     <t>cbs222</t>
   </si>
   <si>
-    <t xml:space="preserve">Criptyk </t>
+    <t>Criptyk</t>
+  </si>
+  <si>
+    <t>sodandy</t>
   </si>
   <si>
     <t>Delsaro</t>
@@ -220,10 +265,10 @@
     <t>dennymane</t>
   </si>
   <si>
-    <t>Dream1528</t>
-  </si>
-  <si>
-    <t>Elizzyble</t>
+    <t>dudeshutup</t>
+  </si>
+  <si>
+    <t>Apix</t>
   </si>
   <si>
     <t>Exenith</t>
@@ -238,13 +283,19 @@
     <t>guergs</t>
   </si>
   <si>
+    <t>NotZyhra</t>
+  </si>
+  <si>
     <t>wonderdogman</t>
   </si>
   <si>
+    <t>diegoz366</t>
+  </si>
+  <si>
     <t>kami_g</t>
   </si>
   <si>
-    <t>Kilthemall</t>
+    <t>kohnja</t>
   </si>
   <si>
     <t>lazyhuy</t>
@@ -256,16 +307,28 @@
     <t>Misha</t>
   </si>
   <si>
+    <t>Mrclutchcakes</t>
+  </si>
+  <si>
+    <t>majesticmikeru</t>
+  </si>
+  <si>
     <t>gizzbro</t>
   </si>
   <si>
     <t>Netninja543</t>
   </si>
   <si>
+    <t>Born8</t>
+  </si>
+  <si>
     <t>Munchy</t>
   </si>
   <si>
-    <t>flyingbeast223</t>
+    <t>partykat</t>
+  </si>
+  <si>
+    <t>Ruekure</t>
   </si>
   <si>
     <t>Ryuden</t>
@@ -280,28 +343,34 @@
     <t>Emperor</t>
   </si>
   <si>
-    <t>plvgrizzly</t>
-  </si>
-  <si>
     <t>Maalinko174</t>
   </si>
   <si>
     <t>SwagPlay</t>
   </si>
   <si>
+    <t>vl_sxicidal_lv</t>
+  </si>
+  <si>
     <t>JustSwift</t>
   </si>
   <si>
     <t>KailyKail</t>
   </si>
   <si>
+    <t>fangednoumenon</t>
+  </si>
+  <si>
+    <t>theethirdman</t>
+  </si>
+  <si>
     <t>TheZeroMark</t>
   </si>
   <si>
     <t>Vasi</t>
   </si>
   <si>
-    <t>Ukass</t>
+    <t>Naut</t>
   </si>
   <si>
     <t>__int3</t>
@@ -319,12 +388,21 @@
     <t>WickedKiss</t>
   </si>
   <si>
+    <t>limis2041</t>
+  </si>
+  <si>
     <t>yami.0</t>
   </si>
   <si>
+    <t>Yamul</t>
+  </si>
+  <si>
     <t>Zednel</t>
   </si>
   <si>
+    <t>mikegangel</t>
+  </si>
+  <si>
     <t>zozrog</t>
   </si>
   <si>
@@ -337,19 +415,22 @@
     <t>banesy</t>
   </si>
   <si>
-    <t>BreninFae</t>
-  </si>
-  <si>
-    <t>Cairis</t>
+    <t>Billberry</t>
+  </si>
+  <si>
+    <t>Cabbit</t>
   </si>
   <si>
     <t>Cenico</t>
   </si>
   <si>
+    <t>Dandyy</t>
+  </si>
+  <si>
     <t>Dennymane</t>
   </si>
   <si>
-    <t>Dreamxx</t>
+    <t>Eiias</t>
   </si>
   <si>
     <t>Flame_Haze</t>
@@ -358,9 +439,15 @@
     <t>Guergs</t>
   </si>
   <si>
+    <t>HanimeDiplomat</t>
+  </si>
+  <si>
     <t>Hooge</t>
   </si>
   <si>
+    <t>IIFrostyII</t>
+  </si>
+  <si>
     <t>KamiG</t>
   </si>
   <si>
@@ -370,13 +457,22 @@
     <t>Mishailia</t>
   </si>
   <si>
+    <t>MrClutchCakes</t>
+  </si>
+  <si>
+    <t>Mykehru</t>
+  </si>
+  <si>
     <t>Naples</t>
   </si>
   <si>
+    <t>Nightmvre</t>
+  </si>
+  <si>
     <t>notmunchy</t>
   </si>
   <si>
-    <t>Ooflegend</t>
+    <t>PartyKat</t>
   </si>
   <si>
     <t>Segwarides</t>
@@ -385,21 +481,27 @@
     <t>Shimhyangje</t>
   </si>
   <si>
-    <t>SilkyRoad</t>
-  </si>
-  <si>
     <t>Sparten</t>
   </si>
   <si>
+    <t>SwearShe18</t>
+  </si>
+  <si>
     <t>Swiftus</t>
   </si>
   <si>
     <t>Talenvard</t>
   </si>
   <si>
+    <t>Taunt</t>
+  </si>
+  <si>
     <t>Thorn_Ess</t>
   </si>
   <si>
+    <t>Tide</t>
+  </si>
+  <si>
     <t>UpCat</t>
   </si>
   <si>
@@ -409,40 +511,55 @@
     <t>Wicked_Kiss</t>
   </si>
   <si>
+    <t>Works</t>
+  </si>
+  <si>
     <t>YA_Mii</t>
   </si>
   <si>
     <t>Zednelem</t>
   </si>
   <si>
+    <t>ZER0420</t>
+  </si>
+  <si>
     <t>Zozrog</t>
   </si>
   <si>
+    <t>Sage</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>Striker</t>
+  </si>
+  <si>
+    <t>Musa</t>
+  </si>
+  <si>
+    <t>Seraph</t>
+  </si>
+  <si>
+    <t>Tamer</t>
+  </si>
+  <si>
+    <t>Dark Knight</t>
+  </si>
+  <si>
+    <t>Sorceress</t>
+  </si>
+  <si>
     <t>Dosa</t>
   </si>
   <si>
-    <t>Witch</t>
-  </si>
-  <si>
-    <t>Striker</t>
-  </si>
-  <si>
-    <t>Seraph</t>
-  </si>
-  <si>
-    <t>Sorceress</t>
-  </si>
-  <si>
-    <t>Dark Knight</t>
-  </si>
-  <si>
     <t>Scholar</t>
   </si>
   <si>
     <t>Ninja</t>
   </si>
   <si>
-    <t>Wizard</t>
+    <t>Ranger</t>
   </si>
   <si>
     <t>Shai</t>
@@ -463,12 +580,12 @@
     <t>Valkyrie</t>
   </si>
   <si>
+    <t>Nova</t>
+  </si>
+  <si>
     <t>Corsair</t>
   </si>
   <si>
-    <t>Musa</t>
-  </si>
-  <si>
     <t>Lahn</t>
   </si>
   <si>
@@ -481,97 +598,100 @@
     <t>Drakania</t>
   </si>
   <si>
-    <t>Ranger</t>
+    <t>Berserker</t>
   </si>
   <si>
     <t>Archer</t>
   </si>
   <si>
-    <t>Berserker</t>
-  </si>
-  <si>
-    <t>Nova</t>
+    <t>Flex</t>
+  </si>
+  <si>
+    <t>Defense, Shai</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Elephant, Scout</t>
+  </si>
+  <si>
+    <t>Offense, Flex</t>
+  </si>
+  <si>
+    <t>Offense, Cannoneer</t>
   </si>
   <si>
     <t>Offense</t>
   </si>
   <si>
-    <t>Defense, Shai</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Elephant, Scout</t>
-  </si>
-  <si>
-    <t>Offense, Flex</t>
-  </si>
-  <si>
-    <t>Flex, Flag Placer</t>
-  </si>
-  <si>
     <t>Offense, Flex, Scout, Flag Placer</t>
   </si>
   <si>
+    <t>Offense, Flex, Elephant, Shotcaller</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Cannoneer, Scout, Flag Placer</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Elephant, Cross comms</t>
+  </si>
+  <si>
+    <t>Defense, Flex, Elephant</t>
+  </si>
+  <si>
+    <t>Shotcaller</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Elephant, Cannoneer, Scout, Flag Placer, Shai, Shotcaller</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Scout</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Cannoneer, Scout, Flag Placer, Shai</t>
+  </si>
+  <si>
+    <t>Offense, Scout</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Elephant, Cannoneer, Scout, Cross comms, Flag Placer, Shotcaller</t>
+  </si>
+  <si>
     <t>Offense, Shotcaller</t>
   </si>
   <si>
-    <t>Defense, Elephant, Shai</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Cannoneer, Scout, Flag Placer</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Elephant, Cross comms</t>
-  </si>
-  <si>
-    <t>Defense, Flex, Elephant</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Shotcaller</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Cannoneer, Scout</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Scout</t>
-  </si>
-  <si>
-    <t>Offense, Scout</t>
-  </si>
-  <si>
-    <t>Offense, Defense, Flex, Scout, Shotcaller</t>
-  </si>
-  <si>
     <t>Offense, Flex, Cannoneer</t>
   </si>
   <si>
     <t>Offense, Defense, Flex, Elephant</t>
   </si>
   <si>
+    <t>Defense, Flex</t>
+  </si>
+  <si>
+    <t>Offense, Flex, Flag Placer</t>
+  </si>
+  <si>
+    <t>Offense, Defense</t>
+  </si>
+  <si>
     <t>Offense, Flex, Scout</t>
   </si>
   <si>
-    <t>Defense, Flex</t>
-  </si>
-  <si>
-    <t>Offense, Flex, Flag Placer</t>
-  </si>
-  <si>
     <t>Defense, Flex, Cannoneer, Scout</t>
   </si>
   <si>
-    <t>Offense, Defense, Elephant, Cannoneer, Shai</t>
-  </si>
-  <si>
     <t>Offense, Defense, Flex, Cannoneer</t>
   </si>
   <si>
+    <t>Offense, Defense, Elephant, Shai</t>
+  </si>
+  <si>
     <t>Offense, Defense, Flex, Elephant, Cannoneer</t>
   </si>
   <si>
     <t>Defense, Elephant</t>
   </si>
   <si>
-    <t>Offense, Defense, Flex, Cannoneer, Scout, Cross comms, Flag Placer</t>
+    <t>Offense, Flex, Cannoneer, Scout, Cross comms, Flag Placer</t>
   </si>
   <si>
     <t>Yes</t>
@@ -935,7 +1055,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -984,13 +1104,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="E2">
         <v>392</v>
@@ -999,22 +1119,22 @@
         <v>388</v>
       </c>
       <c r="G2">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="H2" t="s">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="I2" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="J2" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K2" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L2">
-        <v>849</v>
+        <v>852</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1022,13 +1142,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E3">
         <v>322</v>
@@ -1040,16 +1160,16 @@
         <v>424</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J3" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K3" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="L3">
         <v>751</v>
@@ -1060,13 +1180,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="E4">
         <v>351</v>
@@ -1078,16 +1198,16 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J4" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K4" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L4">
         <v>780</v>
@@ -1098,37 +1218,37 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="E5">
-        <v>347</v>
+        <v>300</v>
       </c>
       <c r="F5">
-        <v>347</v>
+        <v>304</v>
       </c>
       <c r="G5">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="I5" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K5" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L5">
-        <v>773</v>
+        <v>721</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1136,37 +1256,37 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="E6">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F6">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G6">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="I6" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J6" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K6" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L6">
-        <v>780</v>
+        <v>773</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1174,37 +1294,37 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="E7">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F7">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="G7">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="I7" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J7" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K7" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L7">
-        <v>814</v>
+        <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1212,37 +1332,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="E8">
-        <v>358</v>
+        <v>377</v>
       </c>
       <c r="F8">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="G8">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="I8" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K8" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="L8">
-        <v>794</v>
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1250,37 +1370,37 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="E9">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="F9">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="G9">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H9" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="I9" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J9" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K9" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L9">
-        <v>761</v>
+        <v>799</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1288,37 +1408,37 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="E10">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="F10">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="G10">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="I10" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K10" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L10">
-        <v>771</v>
+        <v>794</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1326,37 +1446,37 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="E11">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="F11">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="G11">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="I11" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="J11" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="K11" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L11">
-        <v>841</v>
+        <v>857</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1364,37 +1484,37 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="E12">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="F12">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="G12">
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="I12" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J12" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K12" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L12">
-        <v>781</v>
+        <v>792</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1402,37 +1522,37 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="E13">
-        <v>285</v>
+        <v>385</v>
       </c>
       <c r="F13">
-        <v>287</v>
+        <v>389</v>
       </c>
       <c r="G13">
-        <v>379</v>
+        <v>458</v>
       </c>
       <c r="H13" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="I13" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J13" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K13" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L13">
-        <v>666</v>
+        <v>847</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1440,34 +1560,34 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="E14">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="F14">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="G14">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="I14" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J14" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K14" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L14">
         <v>798</v>
@@ -1478,37 +1598,37 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="E15">
-        <v>389</v>
+        <v>317</v>
       </c>
       <c r="F15">
-        <v>389</v>
+        <v>336</v>
       </c>
       <c r="G15">
-        <v>460</v>
+        <v>415</v>
       </c>
       <c r="H15" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="I15" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J15" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="K15" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L15">
-        <v>849</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1516,37 +1636,37 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="E16">
-        <v>393</v>
+        <v>364</v>
       </c>
       <c r="F16">
-        <v>395</v>
+        <v>342</v>
       </c>
       <c r="G16">
-        <v>463</v>
+        <v>434</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="I16" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="J16" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K16" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L16">
-        <v>858</v>
+        <v>798</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1554,37 +1674,37 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="E17">
         <v>389</v>
       </c>
       <c r="F17">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="G17">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H17" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="I17" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J17" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="K17" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L17">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1592,37 +1712,37 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="E18">
-        <v>282</v>
+        <v>393</v>
       </c>
       <c r="F18">
-        <v>275</v>
+        <v>395</v>
       </c>
       <c r="G18">
-        <v>369</v>
+        <v>463</v>
       </c>
       <c r="H18" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="I18" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J18" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K18" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L18">
-        <v>651</v>
+        <v>858</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1630,37 +1750,37 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="E19">
-        <v>256</v>
+        <v>389</v>
       </c>
       <c r="F19">
-        <v>266</v>
+        <v>393</v>
       </c>
       <c r="G19">
-        <v>317</v>
+        <v>459</v>
       </c>
       <c r="H19" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="I19" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J19" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K19" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="L19">
-        <v>583</v>
+        <v>852</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1668,37 +1788,37 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="E20">
-        <v>390</v>
+        <v>345</v>
       </c>
       <c r="F20">
-        <v>382</v>
+        <v>345</v>
       </c>
       <c r="G20">
-        <v>459</v>
+        <v>396</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="I20" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J20" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K20" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L20">
-        <v>849</v>
+        <v>741</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1706,37 +1826,37 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="E21">
-        <v>374</v>
+        <v>282</v>
       </c>
       <c r="F21">
-        <v>370</v>
+        <v>275</v>
       </c>
       <c r="G21">
-        <v>447</v>
+        <v>369</v>
       </c>
       <c r="H21" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="I21" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J21" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="K21" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L21">
-        <v>821</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1744,37 +1864,37 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="E22">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="F22">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G22">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H22" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="I22" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J22" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K22" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L22">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1782,37 +1902,37 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="E23">
-        <v>365</v>
+        <v>256</v>
       </c>
       <c r="F23">
-        <v>330</v>
+        <v>266</v>
       </c>
       <c r="G23">
-        <v>413</v>
+        <v>317</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="I23" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J23" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K23" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L23">
-        <v>778</v>
+        <v>583</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1820,37 +1940,37 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="E24">
-        <v>386</v>
+        <v>330</v>
       </c>
       <c r="F24">
-        <v>394</v>
+        <v>325</v>
       </c>
       <c r="G24">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="H24" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="I24" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J24" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K24" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L24">
-        <v>856</v>
+        <v>749</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1858,37 +1978,37 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="E25">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="F25">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="G25">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="H25" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="I25" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J25" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="K25" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L25">
-        <v>804</v>
+        <v>818</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1896,37 +2016,37 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="E26">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F26">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G26">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="H26" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
       <c r="I26" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J26" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K26" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="L26">
-        <v>821</v>
+        <v>806</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1934,37 +2054,37 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="D27" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="E27">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="F27">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="G27">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="H27" t="s">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="I27" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J27" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K27" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L27">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1972,37 +2092,37 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="E28">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="F28">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="G28">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="H28" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
       <c r="I28" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J28" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K28" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L28">
-        <v>838</v>
+        <v>860</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2010,37 +2130,37 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="E29">
-        <v>370</v>
+        <v>317</v>
       </c>
       <c r="F29">
-        <v>378</v>
+        <v>322</v>
       </c>
       <c r="G29">
-        <v>437</v>
+        <v>385</v>
       </c>
       <c r="H29" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="I29" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J29" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K29" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L29">
-        <v>815</v>
+        <v>707</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2048,37 +2168,37 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="E30">
-        <v>347</v>
+        <v>386</v>
       </c>
       <c r="F30">
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="G30">
-        <v>435</v>
+        <v>462</v>
       </c>
       <c r="H30" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="I30" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J30" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K30" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L30">
-        <v>798</v>
+        <v>856</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2086,37 +2206,37 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="E31">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F31">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G31">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="I31" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J31" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K31" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L31">
-        <v>823</v>
+        <v>806</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2124,37 +2244,37 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="E32">
-        <v>279</v>
+        <v>390</v>
       </c>
       <c r="F32">
-        <v>291</v>
+        <v>390</v>
       </c>
       <c r="G32">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="I32" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J32" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K32" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L32">
-        <v>651</v>
+        <v>742</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2162,37 +2282,37 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="E33">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F33">
         <v>375</v>
       </c>
       <c r="G33">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="I33" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J33" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K33" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L33">
-        <v>826</v>
+        <v>821</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2200,37 +2320,37 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="E34">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="F34">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="G34">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="H34" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="I34" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J34" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K34" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="L34">
-        <v>819</v>
+        <v>795</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2238,37 +2358,37 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E35">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F35">
-        <v>389</v>
+        <v>364</v>
       </c>
       <c r="G35">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="H35" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="I35" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J35" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="K35" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L35">
-        <v>840</v>
+        <v>795</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2276,37 +2396,37 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="E36">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="F36">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="G36">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="H36" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="I36" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J36" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="K36" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L36">
-        <v>850</v>
+        <v>838</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2314,37 +2434,37 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="E37">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="F37">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="G37">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="H37" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="I37" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J37" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K37" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L37">
-        <v>786</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2352,37 +2472,37 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E38">
-        <v>305</v>
+        <v>347</v>
       </c>
       <c r="F38">
-        <v>307</v>
+        <v>363</v>
       </c>
       <c r="G38">
-        <v>375</v>
+        <v>440</v>
       </c>
       <c r="H38" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="I38" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J38" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K38" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L38">
-        <v>682</v>
+        <v>803</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2390,37 +2510,37 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="E39">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F39">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="G39">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="H39" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="I39" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J39" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K39" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L39">
-        <v>809</v>
+        <v>823</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2428,37 +2548,37 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="E40">
-        <v>332</v>
+        <v>373</v>
       </c>
       <c r="F40">
-        <v>316</v>
+        <v>375</v>
       </c>
       <c r="G40">
-        <v>427</v>
+        <v>451</v>
       </c>
       <c r="H40" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="I40" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J40" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K40" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L40">
-        <v>759</v>
+        <v>826</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2466,37 +2586,37 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="E41">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F41">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="G41">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H41" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="I41" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J41" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K41" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L41">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2504,37 +2624,37 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="E42">
-        <v>374</v>
+        <v>279</v>
       </c>
       <c r="F42">
-        <v>368</v>
+        <v>281</v>
       </c>
       <c r="G42">
-        <v>443</v>
+        <v>369</v>
       </c>
       <c r="H42" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="I42" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J42" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="K42" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L42">
-        <v>817</v>
+        <v>650</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2542,37 +2662,37 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E43">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="F43">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="G43">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="H43" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="I43" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="J43" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="K43" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L43">
-        <v>818</v>
+        <v>842</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2580,37 +2700,37 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="E44">
-        <v>342</v>
+        <v>390</v>
       </c>
       <c r="F44">
-        <v>342</v>
+        <v>390</v>
       </c>
       <c r="G44">
-        <v>416</v>
+        <v>460</v>
       </c>
       <c r="H44" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="I44" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J44" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="K44" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L44">
-        <v>758</v>
+        <v>850</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2618,37 +2738,37 @@
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="E45">
-        <v>318</v>
+        <v>373</v>
       </c>
       <c r="F45">
-        <v>322</v>
+        <v>373</v>
       </c>
       <c r="G45">
-        <v>314</v>
+        <v>440</v>
       </c>
       <c r="H45" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="I45" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J45" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K45" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="L45">
-        <v>636</v>
+        <v>813</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2656,37 +2776,37 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="E46">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="F46">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="G46">
-        <v>411</v>
+        <v>438</v>
       </c>
       <c r="H46" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="I46" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J46" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="K46" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="L46">
-        <v>749</v>
+        <v>806</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2694,13 +2814,13 @@
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="E47">
         <v>358</v>
@@ -2709,22 +2829,516 @@
         <v>358</v>
       </c>
       <c r="G47">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="H47" t="s">
+        <v>199</v>
+      </c>
+      <c r="I47" t="s">
+        <v>227</v>
+      </c>
+      <c r="J47" t="s">
+        <v>227</v>
+      </c>
+      <c r="K47" t="s">
+        <v>226</v>
+      </c>
+      <c r="L47">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48">
+        <v>305</v>
+      </c>
+      <c r="F48">
+        <v>307</v>
+      </c>
+      <c r="G48">
+        <v>375</v>
+      </c>
+      <c r="H48" t="s">
+        <v>220</v>
+      </c>
+      <c r="I48" t="s">
+        <v>227</v>
+      </c>
+      <c r="J48" t="s">
+        <v>227</v>
+      </c>
+      <c r="K48" t="s">
+        <v>226</v>
+      </c>
+      <c r="L48">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49">
+        <v>390</v>
+      </c>
+      <c r="F49">
+        <v>394</v>
+      </c>
+      <c r="G49">
+        <v>464</v>
+      </c>
+      <c r="H49" t="s">
+        <v>201</v>
+      </c>
+      <c r="I49" t="s">
+        <v>226</v>
+      </c>
+      <c r="J49" t="s">
+        <v>227</v>
+      </c>
+      <c r="K49" t="s">
+        <v>226</v>
+      </c>
+      <c r="L49">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50">
+        <v>332</v>
+      </c>
+      <c r="F50">
+        <v>316</v>
+      </c>
+      <c r="G50">
+        <v>427</v>
+      </c>
+      <c r="H50" t="s">
+        <v>221</v>
+      </c>
+      <c r="I50" t="s">
+        <v>227</v>
+      </c>
+      <c r="J50" t="s">
+        <v>227</v>
+      </c>
+      <c r="K50" t="s">
+        <v>226</v>
+      </c>
+      <c r="L50">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51">
+        <v>377</v>
+      </c>
+      <c r="F51">
+        <v>383</v>
+      </c>
+      <c r="G51">
+        <v>443</v>
+      </c>
+      <c r="H51" t="s">
+        <v>199</v>
+      </c>
+      <c r="I51" t="s">
+        <v>226</v>
+      </c>
+      <c r="J51" t="s">
+        <v>227</v>
+      </c>
+      <c r="K51" t="s">
+        <v>227</v>
+      </c>
+      <c r="L51">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52">
+        <v>381</v>
+      </c>
+      <c r="F52">
+        <v>377</v>
+      </c>
+      <c r="G52">
+        <v>443</v>
+      </c>
+      <c r="H52" t="s">
+        <v>222</v>
+      </c>
+      <c r="I52" t="s">
+        <v>227</v>
+      </c>
+      <c r="J52" t="s">
+        <v>226</v>
+      </c>
+      <c r="K52" t="s">
+        <v>226</v>
+      </c>
+      <c r="L52">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" t="s">
+        <v>171</v>
+      </c>
+      <c r="E53">
+        <v>381</v>
+      </c>
+      <c r="F53">
+        <v>381</v>
+      </c>
+      <c r="G53">
+        <v>444</v>
+      </c>
+      <c r="H53" t="s">
+        <v>201</v>
+      </c>
+      <c r="I53" t="s">
+        <v>227</v>
+      </c>
+      <c r="J53" t="s">
+        <v>227</v>
+      </c>
+      <c r="K53" t="s">
+        <v>226</v>
+      </c>
+      <c r="L53">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54">
+        <v>354</v>
+      </c>
+      <c r="F54">
+        <v>354</v>
+      </c>
+      <c r="G54">
+        <v>430</v>
+      </c>
+      <c r="H54" t="s">
+        <v>223</v>
+      </c>
+      <c r="I54" t="s">
+        <v>227</v>
+      </c>
+      <c r="J54" t="s">
+        <v>226</v>
+      </c>
+      <c r="K54" t="s">
+        <v>226</v>
+      </c>
+      <c r="L54">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55" t="s">
+        <v>194</v>
+      </c>
+      <c r="E55">
+        <v>305</v>
+      </c>
+      <c r="F55">
+        <v>296</v>
+      </c>
+      <c r="G55">
+        <v>386</v>
+      </c>
+      <c r="H55" t="s">
+        <v>201</v>
+      </c>
+      <c r="I55" t="s">
+        <v>227</v>
+      </c>
+      <c r="J55" t="s">
+        <v>227</v>
+      </c>
+      <c r="K55" t="s">
+        <v>226</v>
+      </c>
+      <c r="L55">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56">
+        <v>318</v>
+      </c>
+      <c r="F56">
+        <v>322</v>
+      </c>
+      <c r="G56">
+        <v>314</v>
+      </c>
+      <c r="H56" t="s">
+        <v>224</v>
+      </c>
+      <c r="I56" t="s">
+        <v>227</v>
+      </c>
+      <c r="J56" t="s">
+        <v>227</v>
+      </c>
+      <c r="K56" t="s">
+        <v>226</v>
+      </c>
+      <c r="L56">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" t="s">
+        <v>184</v>
+      </c>
+      <c r="E57">
+        <v>355</v>
+      </c>
+      <c r="F57">
+        <v>355</v>
+      </c>
+      <c r="G57">
+        <v>428</v>
+      </c>
+      <c r="H57" t="s">
+        <v>201</v>
+      </c>
+      <c r="I57" t="s">
+        <v>227</v>
+      </c>
+      <c r="J57" t="s">
+        <v>227</v>
+      </c>
+      <c r="K57" t="s">
+        <v>226</v>
+      </c>
+      <c r="L57">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58">
+        <v>336</v>
+      </c>
+      <c r="F58">
+        <v>338</v>
+      </c>
+      <c r="G58">
+        <v>411</v>
+      </c>
+      <c r="H58" t="s">
+        <v>201</v>
+      </c>
+      <c r="I58" t="s">
+        <v>227</v>
+      </c>
+      <c r="J58" t="s">
+        <v>227</v>
+      </c>
+      <c r="K58" t="s">
+        <v>226</v>
+      </c>
+      <c r="L58">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" t="s">
         <v>185</v>
       </c>
-      <c r="I47" t="s">
-        <v>186</v>
-      </c>
-      <c r="J47" t="s">
-        <v>186</v>
-      </c>
-      <c r="K47" t="s">
-        <v>187</v>
-      </c>
-      <c r="L47">
-        <v>792</v>
+      <c r="E59">
+        <v>366</v>
+      </c>
+      <c r="F59">
+        <v>366</v>
+      </c>
+      <c r="G59">
+        <v>443</v>
+      </c>
+      <c r="H59" t="s">
+        <v>219</v>
+      </c>
+      <c r="I59" t="s">
+        <v>227</v>
+      </c>
+      <c r="J59" t="s">
+        <v>226</v>
+      </c>
+      <c r="K59" t="s">
+        <v>226</v>
+      </c>
+      <c r="L59">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60">
+        <v>361</v>
+      </c>
+      <c r="F60">
+        <v>361</v>
+      </c>
+      <c r="G60">
+        <v>437</v>
+      </c>
+      <c r="H60" t="s">
+        <v>225</v>
+      </c>
+      <c r="I60" t="s">
+        <v>226</v>
+      </c>
+      <c r="J60" t="s">
+        <v>226</v>
+      </c>
+      <c r="K60" t="s">
+        <v>226</v>
+      </c>
+      <c r="L60">
+        <v>798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a way to update ap dp and aap
</commit_message>
<xml_diff>
--- a/NSguildresponses.xlsx
+++ b/NSguildresponses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="224">
   <si>
     <t>0</t>
   </si>
@@ -55,7 +55,7 @@
     <t>2026-01-21 17:20:55</t>
   </si>
   <si>
-    <t>2025-12-25 02:45:26</t>
+    <t>2026-01-25 17:13:47</t>
   </si>
   <si>
     <t>2026-01-01 17:20:47</t>
@@ -127,7 +127,7 @@
     <t>2026-01-11 12:34:01</t>
   </si>
   <si>
-    <t>2026-01-25 13:35:17</t>
+    <t>2026-01-25 13:54:24</t>
   </si>
   <si>
     <t>2026-01-22 23:53:09</t>
@@ -136,9 +136,6 @@
     <t>2026-01-23 00:12:53</t>
   </si>
   <si>
-    <t>2025-12-25 13:18:12</t>
-  </si>
-  <si>
     <t>2026-01-21 16:47:55</t>
   </si>
   <si>
@@ -232,7 +229,7 @@
     <t>acidfs</t>
   </si>
   <si>
-    <t>brhee_miko.</t>
+    <t>Ayamiko</t>
   </si>
   <si>
     <t>banes</t>
@@ -313,9 +310,6 @@
     <t>majesticmikeru</t>
   </si>
   <si>
-    <t>gizzbro</t>
-  </si>
-  <si>
     <t>Netninja543</t>
   </si>
   <si>
@@ -409,9 +403,6 @@
     <t>AcidFS</t>
   </si>
   <si>
-    <t>Ayamiko</t>
-  </si>
-  <si>
     <t>banesy</t>
   </si>
   <si>
@@ -463,9 +454,6 @@
     <t>Mykehru</t>
   </si>
   <si>
-    <t>Naples</t>
-  </si>
-  <si>
     <t>Nightmvre</t>
   </si>
   <si>
@@ -529,105 +517,108 @@
     <t>Sage</t>
   </si>
   <si>
+    <t>Corsair</t>
+  </si>
+  <si>
+    <t>Striker</t>
+  </si>
+  <si>
+    <t>Musa</t>
+  </si>
+  <si>
+    <t>Seraph</t>
+  </si>
+  <si>
+    <t>Tamer</t>
+  </si>
+  <si>
+    <t>Dark Knight</t>
+  </si>
+  <si>
+    <t>Sorceress</t>
+  </si>
+  <si>
+    <t>Dosa</t>
+  </si>
+  <si>
+    <t>Scholar</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Shai</t>
+  </si>
+  <si>
+    <t>Kunoichi</t>
+  </si>
+  <si>
+    <t>Maegu</t>
+  </si>
+  <si>
+    <t>Hashashin</t>
+  </si>
+  <si>
+    <t>Mystic</t>
+  </si>
+  <si>
+    <t>Valkyrie</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Lahn</t>
+  </si>
+  <si>
+    <t>Maehwa</t>
+  </si>
+  <si>
+    <t>Guardian</t>
+  </si>
+  <si>
+    <t>Drakania</t>
+  </si>
+  <si>
+    <t>Berserker</t>
+  </si>
+  <si>
     <t>Witch</t>
   </si>
   <si>
-    <t>Striker</t>
-  </si>
-  <si>
-    <t>Musa</t>
-  </si>
-  <si>
-    <t>Seraph</t>
-  </si>
-  <si>
-    <t>Tamer</t>
-  </si>
-  <si>
-    <t>Dark Knight</t>
-  </si>
-  <si>
-    <t>Sorceress</t>
-  </si>
-  <si>
-    <t>Dosa</t>
-  </si>
-  <si>
-    <t>Scholar</t>
-  </si>
-  <si>
-    <t>Ninja</t>
-  </si>
-  <si>
-    <t>Ranger</t>
-  </si>
-  <si>
-    <t>Shai</t>
-  </si>
-  <si>
-    <t>Kunoichi</t>
-  </si>
-  <si>
-    <t>Maegu</t>
-  </si>
-  <si>
-    <t>Hashashin</t>
-  </si>
-  <si>
-    <t>Mystic</t>
-  </si>
-  <si>
-    <t>Valkyrie</t>
-  </si>
-  <si>
-    <t>Nova</t>
-  </si>
-  <si>
-    <t>Corsair</t>
-  </si>
-  <si>
-    <t>Lahn</t>
-  </si>
-  <si>
-    <t>Maehwa</t>
-  </si>
-  <si>
-    <t>Guardian</t>
-  </si>
-  <si>
-    <t>Drakania</t>
-  </si>
-  <si>
-    <t>Berserker</t>
-  </si>
-  <si>
     <t>Archer</t>
   </si>
   <si>
     <t>Flex</t>
   </si>
   <si>
+    <t>Offense, Defense, Shai</t>
+  </si>
+  <si>
+    <t>Offense, Defense, Flex, Elephant, Scout</t>
+  </si>
+  <si>
+    <t>Offense, Flex</t>
+  </si>
+  <si>
+    <t>Offense, Cannoneer</t>
+  </si>
+  <si>
+    <t>Offense</t>
+  </si>
+  <si>
+    <t>Offense, Flex, Scout, Flag Placer</t>
+  </si>
+  <si>
+    <t>Offense, Flex, Elephant, Shotcaller</t>
+  </si>
+  <si>
     <t>Defense, Shai</t>
   </si>
   <si>
-    <t>Offense, Defense, Flex, Elephant, Scout</t>
-  </si>
-  <si>
-    <t>Offense, Flex</t>
-  </si>
-  <si>
-    <t>Offense, Cannoneer</t>
-  </si>
-  <si>
-    <t>Offense</t>
-  </si>
-  <si>
-    <t>Offense, Flex, Scout, Flag Placer</t>
-  </si>
-  <si>
-    <t>Offense, Flex, Elephant, Shotcaller</t>
-  </si>
-  <si>
     <t>Offense, Defense, Flex, Cannoneer, Scout, Flag Placer</t>
   </si>
   <si>
@@ -647,9 +638,6 @@
   </si>
   <si>
     <t>Offense, Defense, Flex, Cannoneer, Scout, Flag Placer, Shai</t>
-  </si>
-  <si>
-    <t>Offense, Scout</t>
   </si>
   <si>
     <t>Offense, Defense, Flex, Elephant, Cannoneer, Scout, Cross comms, Flag Placer, Shotcaller</t>
@@ -1055,7 +1043,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1104,13 +1092,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E2">
         <v>392</v>
@@ -1122,16 +1110,16 @@
         <v>460</v>
       </c>
       <c r="H2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L2">
         <v>852</v>
@@ -1142,37 +1130,37 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E3">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="F3">
         <v>327</v>
       </c>
       <c r="G3">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="H3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L3">
-        <v>751</v>
+        <v>756</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1180,13 +1168,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E4">
         <v>351</v>
@@ -1198,16 +1186,16 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L4">
         <v>780</v>
@@ -1218,13 +1206,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E5">
         <v>300</v>
@@ -1236,16 +1224,16 @@
         <v>417</v>
       </c>
       <c r="H5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L5">
         <v>721</v>
@@ -1256,13 +1244,13 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E6">
         <v>347</v>
@@ -1274,16 +1262,16 @@
         <v>426</v>
       </c>
       <c r="H6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L6">
         <v>773</v>
@@ -1294,13 +1282,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E7">
         <v>371</v>
@@ -1312,16 +1300,16 @@
         <v>425</v>
       </c>
       <c r="H7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L7">
         <v>800</v>
@@ -1332,13 +1320,13 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E8">
         <v>377</v>
@@ -1350,16 +1338,16 @@
         <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L8">
         <v>821</v>
@@ -1370,13 +1358,13 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E9">
         <v>367</v>
@@ -1388,16 +1376,16 @@
         <v>428</v>
       </c>
       <c r="H9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L9">
         <v>799</v>
@@ -1408,13 +1396,13 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E10">
         <v>365</v>
@@ -1426,16 +1414,16 @@
         <v>429</v>
       </c>
       <c r="H10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L10">
         <v>794</v>
@@ -1446,13 +1434,13 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E11">
         <v>393</v>
@@ -1464,16 +1452,16 @@
         <v>464</v>
       </c>
       <c r="H11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L11">
         <v>857</v>
@@ -1484,13 +1472,13 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E12">
         <v>365</v>
@@ -1502,16 +1490,16 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L12">
         <v>792</v>
@@ -1522,16 +1510,16 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E13">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="F13">
         <v>389</v>
@@ -1540,16 +1528,16 @@
         <v>458</v>
       </c>
       <c r="H13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J13" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L13">
         <v>847</v>
@@ -1560,13 +1548,13 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E14">
         <v>373</v>
@@ -1578,16 +1566,16 @@
         <v>425</v>
       </c>
       <c r="H14" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K14" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L14">
         <v>798</v>
@@ -1598,13 +1586,13 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E15">
         <v>317</v>
@@ -1616,16 +1604,16 @@
         <v>415</v>
       </c>
       <c r="H15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L15">
         <v>751</v>
@@ -1636,13 +1624,13 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E16">
         <v>364</v>
@@ -1654,16 +1642,16 @@
         <v>434</v>
       </c>
       <c r="H16" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L16">
         <v>798</v>
@@ -1674,13 +1662,13 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E17">
         <v>389</v>
@@ -1692,16 +1680,16 @@
         <v>460</v>
       </c>
       <c r="H17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L17">
         <v>849</v>
@@ -1712,13 +1700,13 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E18">
         <v>393</v>
@@ -1730,16 +1718,16 @@
         <v>463</v>
       </c>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I18" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K18" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L18">
         <v>858</v>
@@ -1750,13 +1738,13 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E19">
         <v>389</v>
@@ -1768,16 +1756,16 @@
         <v>459</v>
       </c>
       <c r="H19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L19">
         <v>852</v>
@@ -1788,13 +1776,13 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E20">
         <v>345</v>
@@ -1806,16 +1794,16 @@
         <v>396</v>
       </c>
       <c r="H20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L20">
         <v>741</v>
@@ -1826,13 +1814,13 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E21">
         <v>282</v>
@@ -1844,16 +1832,16 @@
         <v>369</v>
       </c>
       <c r="H21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I21" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J21" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K21" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L21">
         <v>651</v>
@@ -1864,13 +1852,13 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E22">
         <v>371</v>
@@ -1882,16 +1870,16 @@
         <v>433</v>
       </c>
       <c r="H22" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I22" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J22" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K22" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L22">
         <v>804</v>
@@ -1902,13 +1890,13 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E23">
         <v>256</v>
@@ -1920,16 +1908,16 @@
         <v>317</v>
       </c>
       <c r="H23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I23" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J23" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K23" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L23">
         <v>583</v>
@@ -1940,13 +1928,13 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E24">
         <v>330</v>
@@ -1958,16 +1946,16 @@
         <v>419</v>
       </c>
       <c r="H24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I24" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J24" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K24" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L24">
         <v>749</v>
@@ -1978,13 +1966,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="E25">
         <v>375</v>
@@ -1996,16 +1984,16 @@
         <v>443</v>
       </c>
       <c r="H25" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I25" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J25" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K25" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L25">
         <v>818</v>
@@ -2016,13 +2004,13 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E26">
         <v>368</v>
@@ -2034,16 +2022,16 @@
         <v>433</v>
       </c>
       <c r="H26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I26" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J26" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K26" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L26">
         <v>806</v>
@@ -2054,13 +2042,13 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E27">
         <v>376</v>
@@ -2072,16 +2060,16 @@
         <v>429</v>
       </c>
       <c r="H27" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I27" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J27" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K27" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L27">
         <v>805</v>
@@ -2092,13 +2080,13 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E28">
         <v>395</v>
@@ -2110,16 +2098,16 @@
         <v>465</v>
       </c>
       <c r="H28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I28" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J28" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K28" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -2130,13 +2118,13 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E29">
         <v>317</v>
@@ -2148,16 +2136,16 @@
         <v>385</v>
       </c>
       <c r="H29" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I29" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J29" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K29" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L29">
         <v>707</v>
@@ -2168,37 +2156,37 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E30">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="F30">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="G30">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="H30" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J30" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K30" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L30">
-        <v>856</v>
+        <v>806</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2206,37 +2194,37 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E31">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="F31">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="G31">
-        <v>441</v>
+        <v>352</v>
       </c>
       <c r="H31" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="I31" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J31" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K31" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L31">
-        <v>806</v>
+        <v>742</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2244,37 +2232,37 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E32">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="F32">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="G32">
-        <v>352</v>
+        <v>446</v>
       </c>
       <c r="H32" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="I32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K32" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L32">
-        <v>742</v>
+        <v>821</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2282,37 +2270,37 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D33" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="E33">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F33">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G33">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="H33" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="I33" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J33" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K33" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L33">
-        <v>821</v>
+        <v>795</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2320,34 +2308,34 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E34">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F34">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G34">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H34" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I34" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J34" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K34" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L34">
         <v>795</v>
@@ -2358,37 +2346,37 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E35">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="F35">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="G35">
-        <v>427</v>
+        <v>453</v>
       </c>
       <c r="H35" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="I35" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J35" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K35" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L35">
-        <v>795</v>
+        <v>838</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2396,37 +2384,37 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E36">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="F36">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G36">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="H36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I36" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J36" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K36" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L36">
-        <v>838</v>
+        <v>815</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2434,37 +2422,37 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="D37" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="E37">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="F37">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="G37">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="H37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I37" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J37" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K37" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L37">
-        <v>815</v>
+        <v>803</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2472,37 +2460,37 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E38">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="F38">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="G38">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="H38" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="I38" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J38" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K38" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L38">
-        <v>803</v>
+        <v>823</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2510,37 +2498,37 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E39">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F39">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="G39">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H39" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="I39" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J39" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K39" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L39">
-        <v>823</v>
+        <v>826</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2548,37 +2536,37 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
         <v>180</v>
       </c>
       <c r="E40">
+        <v>379</v>
+      </c>
+      <c r="F40">
         <v>373</v>
       </c>
-      <c r="F40">
-        <v>375</v>
-      </c>
       <c r="G40">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="H40" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I40" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J40" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K40" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L40">
-        <v>826</v>
+        <v>819</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2586,37 +2574,37 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E41">
-        <v>379</v>
+        <v>279</v>
       </c>
       <c r="F41">
-        <v>373</v>
+        <v>281</v>
       </c>
       <c r="G41">
-        <v>440</v>
+        <v>369</v>
       </c>
       <c r="H41" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I41" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J41" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K41" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L41">
-        <v>819</v>
+        <v>650</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2624,37 +2612,37 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E42">
-        <v>279</v>
+        <v>385</v>
       </c>
       <c r="F42">
-        <v>281</v>
+        <v>391</v>
       </c>
       <c r="G42">
-        <v>369</v>
+        <v>451</v>
       </c>
       <c r="H42" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I42" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J42" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K42" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L42">
-        <v>650</v>
+        <v>842</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2662,37 +2650,37 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
         <v>183</v>
       </c>
       <c r="E43">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F43">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G43">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="H43" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I43" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J43" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K43" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L43">
-        <v>842</v>
+        <v>850</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2700,37 +2688,37 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D44" t="s">
         <v>187</v>
       </c>
       <c r="E44">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="F44">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="G44">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="H44" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="I44" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J44" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K44" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L44">
-        <v>850</v>
+        <v>813</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2738,37 +2726,37 @@
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="E45">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F45">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="G45">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H45" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I45" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J45" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K45" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L45">
-        <v>813</v>
+        <v>806</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2776,37 +2764,37 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="E46">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F46">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="G46">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="H46" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I46" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J46" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K46" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L46">
-        <v>806</v>
+        <v>786</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2814,37 +2802,37 @@
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="E47">
-        <v>358</v>
+        <v>305</v>
       </c>
       <c r="F47">
-        <v>358</v>
+        <v>307</v>
       </c>
       <c r="G47">
-        <v>428</v>
+        <v>375</v>
       </c>
       <c r="H47" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="I47" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J47" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K47" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L47">
-        <v>786</v>
+        <v>682</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2852,37 +2840,37 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D48" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E48">
-        <v>305</v>
+        <v>390</v>
       </c>
       <c r="F48">
-        <v>307</v>
+        <v>394</v>
       </c>
       <c r="G48">
-        <v>375</v>
+        <v>464</v>
       </c>
       <c r="H48" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="I48" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J48" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K48" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L48">
-        <v>682</v>
+        <v>858</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2890,37 +2878,37 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D49" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E49">
-        <v>390</v>
+        <v>332</v>
       </c>
       <c r="F49">
-        <v>394</v>
+        <v>316</v>
       </c>
       <c r="G49">
-        <v>464</v>
+        <v>427</v>
       </c>
       <c r="H49" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="I49" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J49" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K49" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L49">
-        <v>858</v>
+        <v>759</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2928,37 +2916,37 @@
         <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="E50">
-        <v>332</v>
+        <v>377</v>
       </c>
       <c r="F50">
-        <v>316</v>
+        <v>383</v>
       </c>
       <c r="G50">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="H50" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="I50" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J50" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K50" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L50">
-        <v>759</v>
+        <v>826</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2966,37 +2954,37 @@
         <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E51">
+        <v>381</v>
+      </c>
+      <c r="F51">
         <v>377</v>
-      </c>
-      <c r="F51">
-        <v>383</v>
       </c>
       <c r="G51">
         <v>443</v>
       </c>
       <c r="H51" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="I51" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J51" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K51" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L51">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3004,37 +2992,37 @@
         <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="D52" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E52">
         <v>381</v>
       </c>
       <c r="F52">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="G52">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H52" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="I52" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J52" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K52" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L52">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3042,37 +3030,37 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="E53">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="F53">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="G53">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="H53" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="I53" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J53" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K53" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L53">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3080,37 +3068,37 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E54">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="F54">
-        <v>354</v>
+        <v>296</v>
       </c>
       <c r="G54">
-        <v>430</v>
+        <v>386</v>
       </c>
       <c r="H54" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="I54" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J54" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K54" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L54">
-        <v>784</v>
+        <v>691</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3118,37 +3106,37 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E55">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="F55">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="G55">
-        <v>386</v>
+        <v>314</v>
       </c>
       <c r="H55" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="I55" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J55" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K55" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L55">
-        <v>691</v>
+        <v>636</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3156,37 +3144,37 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E56">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F56">
-        <v>322</v>
+        <v>355</v>
       </c>
       <c r="G56">
-        <v>314</v>
+        <v>428</v>
       </c>
       <c r="H56" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="I56" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J56" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K56" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L56">
-        <v>636</v>
+        <v>783</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3194,37 +3182,37 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="E57">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="F57">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="G57">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="H57" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I57" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J57" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K57" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L57">
-        <v>783</v>
+        <v>749</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3232,37 +3220,37 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E58">
-        <v>336</v>
+        <v>366</v>
       </c>
       <c r="F58">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="G58">
-        <v>411</v>
+        <v>443</v>
       </c>
       <c r="H58" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="I58" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J58" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K58" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L58">
-        <v>749</v>
+        <v>809</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3270,74 +3258,36 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D59" t="s">
         <v>185</v>
       </c>
       <c r="E59">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F59">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G59">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="H59" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I59" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J59" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K59" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L59">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>129</v>
-      </c>
-      <c r="C60" t="s">
-        <v>169</v>
-      </c>
-      <c r="D60" t="s">
-        <v>190</v>
-      </c>
-      <c r="E60">
-        <v>361</v>
-      </c>
-      <c r="F60">
-        <v>361</v>
-      </c>
-      <c r="G60">
-        <v>437</v>
-      </c>
-      <c r="H60" t="s">
-        <v>225</v>
-      </c>
-      <c r="I60" t="s">
-        <v>226</v>
-      </c>
-      <c r="J60" t="s">
-        <v>226</v>
-      </c>
-      <c r="K60" t="s">
-        <v>226</v>
-      </c>
-      <c r="L60">
         <v>798</v>
       </c>
     </row>

</xml_diff>